<commit_message>
Major Update. Traceability Matrix Template.xls update code descripcion, code update but keeps doing weird things in antipinch.
</commit_message>
<xml_diff>
--- a/V Cycle Process/Defect Log.xlsx
+++ b/V Cycle Process/Defect Log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="7815"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Defect logs " sheetId="1" r:id="rId1"/>
@@ -239,8 +239,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,6 +826,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -908,6 +913,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -942,6 +948,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1117,14 +1124,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
@@ -1139,7 +1146,7 @@
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1165,7 +1172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1175,7 +1182,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1185,7 +1192,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1195,7 +1202,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1205,7 +1212,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1215,7 +1222,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1225,7 +1232,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1235,7 +1242,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1245,7 +1252,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1255,7 +1262,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1265,7 +1272,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1275,7 +1282,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1285,7 +1292,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1295,7 +1302,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1305,7 +1312,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1315,7 +1322,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1325,7 +1332,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1335,7 +1342,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1345,7 +1352,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1355,7 +1362,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1365,7 +1372,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1375,7 +1382,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1385,7 +1392,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1395,7 +1402,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1405,7 +1412,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1415,7 +1422,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1425,7 +1432,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1435,7 +1442,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1445,7 +1452,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1462,20 +1469,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30">
+    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1499,7 +1506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="30">
+    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="30">
+    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1515,7 +1522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="30">
+    <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1523,7 +1530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1531,7 +1538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1539,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="30">
+    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1555,7 +1562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="30">
+    <row r="14" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Added Diagrams to Design Template.
</commit_message>
<xml_diff>
--- a/V Cycle Process/Defect Log.xlsx
+++ b/V Cycle Process/Defect Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Defect logs " sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -234,6 +234,33 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Windowlifter.c</t>
+  </si>
+  <si>
+    <t>Enviroment</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
+    <t>The uC is not respecting the order of the functions and is executing in aleatory order.</t>
+  </si>
+  <si>
+    <t>Windowlifter.h</t>
+  </si>
+  <si>
+    <t>Duplicate declaration, variable and function.</t>
+  </si>
+  <si>
+    <t>main.c</t>
+  </si>
+  <si>
+    <t>Added c templated and function descriptions.</t>
   </si>
 </sst>
 </file>
@@ -767,7 +794,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -778,6 +805,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1127,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1168,7 @@
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="7" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="36.140625" customWidth="1"/>
@@ -1172,35 +1203,83 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5">
+        <v>42188</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5">
+        <v>42188</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42188</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
@@ -1210,7 +1289,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
@@ -1220,7 +1299,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
@@ -1230,7 +1309,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
@@ -1240,7 +1319,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
@@ -1250,7 +1329,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -1260,7 +1339,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
@@ -1270,7 +1349,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
@@ -1280,7 +1359,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
@@ -1290,7 +1369,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -1300,7 +1379,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
@@ -1310,7 +1389,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
@@ -1320,7 +1399,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
@@ -1330,7 +1409,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
@@ -1340,7 +1419,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
@@ -1350,7 +1429,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
@@ -1360,7 +1439,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
@@ -1370,7 +1449,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
@@ -1380,7 +1459,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
@@ -1390,7 +1469,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
@@ -1400,7 +1479,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="6"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
@@ -1410,7 +1489,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="6"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
@@ -1420,7 +1499,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="6"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
@@ -1430,7 +1509,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="6"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
@@ -1440,7 +1519,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="I30" s="6"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
@@ -1450,7 +1529,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="I31" s="6"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
@@ -1460,11 +1539,12 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1472,9 +1552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>